<commit_message>
added initial script to generate at commands, but still incomplete
</commit_message>
<xml_diff>
--- a/tests/menubar-editor/data/200130_Menubar_test writing.xlsx
+++ b/tests/menubar-editor/data/200130_Menubar_test writing.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89E52F44-0535-4F7D-973A-D3B090750630}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B48A7F21-F296-49AE-877A-99B5964D16CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1433" windowWidth="25110" windowHeight="13957" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2483" yWindow="2483" windowWidth="21600" windowHeight="11422" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="5" r:id="rId1"/>
@@ -297,37 +297,37 @@
     <t>jaws</t>
   </si>
   <si>
-    <t>Enter</t>
-  </si>
-  <si>
-    <t>Tab / Shift+Tab</t>
-  </si>
-  <si>
-    <t>F/Shift+F</t>
-  </si>
-  <si>
-    <t>Up Arrow / Down Arrow</t>
-  </si>
-  <si>
-    <t>Left Arrow / Right Arrow (with Smart Navigation on)</t>
-  </si>
-  <si>
-    <t>S(Navigate by first letter of menuitem)</t>
-  </si>
-  <si>
-    <t>B(Navigate by first letter of menuitem)</t>
-  </si>
-  <si>
-    <t>Space</t>
-  </si>
-  <si>
-    <t>Esc</t>
-  </si>
-  <si>
-    <t>Insert+Tab (or CapsLock+Tab)</t>
-  </si>
-  <si>
-    <t>Insert+Up (or CapsLock+I)</t>
+    <t>ENTER</t>
+  </si>
+  <si>
+    <t>TAB_AND_SHIFT_TAB</t>
+  </si>
+  <si>
+    <t>F_AND_SHIFT_F</t>
+  </si>
+  <si>
+    <t>UP_AND_DOWN</t>
+  </si>
+  <si>
+    <t>LEFT_AND_RIGHT (with Smart Navigation on)</t>
+  </si>
+  <si>
+    <t>S (Navigate by first letter of menuitem)</t>
+  </si>
+  <si>
+    <t>B (Navigate by first letter of menuitem)</t>
+  </si>
+  <si>
+    <t>SPACE</t>
+  </si>
+  <si>
+    <t>ESC</t>
+  </si>
+  <si>
+    <t>INSERT_TAB</t>
+  </si>
+  <si>
+    <t>INSERT_UP</t>
   </si>
   <si>
     <t>Pattern Name:</t>
@@ -1344,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB114850-8975-4895-822B-FAA214380FDD}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2145,8 +2145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD08FFF1-5FCA-4B3E-93F6-A3BD4D87742D}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>